<commit_message>
Last check by me and edited some of the format and visual style for all excel files
</commit_message>
<xml_diff>
--- a/Phase 2/burndown chart.xlsx
+++ b/Phase 2/burndown chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="165" windowWidth="17235" windowHeight="8895"/>
+    <workbookView xWindow="120" yWindow="168" windowWidth="17232" windowHeight="8892"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,11 +94,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -106,7 +106,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -114,16 +114,43 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -165,21 +192,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="差" xfId="2" builtinId="27"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -194,7 +224,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="ko-KR"/>
+  <c:lang val="en-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -312,8 +342,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="44751104"/>
-        <c:axId val="45220224"/>
+        <c:axId val="125196160"/>
+        <c:axId val="125198336"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -525,11 +555,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44751104"/>
-        <c:axId val="45220224"/>
+        <c:axId val="125196160"/>
+        <c:axId val="125198336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44751104"/>
+        <c:axId val="125196160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,7 +587,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45220224"/>
+        <c:crossAx val="125198336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -565,7 +595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45220224"/>
+        <c:axId val="125198336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,7 +625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44751104"/>
+        <c:crossAx val="125196160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -659,7 +689,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -948,22 +978,22 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="F9" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
-    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
-    <col min="6" max="6" width="31.625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1">
@@ -977,19 +1007,19 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1094,19 +1124,19 @@
       <c r="E9">
         <v>77</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1126,7 +1156,7 @@
       <c r="E10">
         <v>74</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H10">
@@ -1507,7 +1537,8 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1517,7 +1548,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1530,7 +1561,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>